<commit_message>
basic tensorflow code and update workSheet
</commit_message>
<xml_diff>
--- a/workSheet.xlsx
+++ b/workSheet.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F53C2CA4-BD42-4224-B6C1-603BB40001B6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="2070" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="13">
   <si>
     <t>วันที่</t>
   </si>
@@ -51,13 +52,19 @@
     <t>-origin : https://github.com/santainw/textBaseMiningOfServiceFeedBack.git</t>
   </si>
   <si>
-    <t>Upload_Paper_Thai</t>
+    <t>2.Upload_Paper_Thai</t>
+  </si>
+  <si>
+    <t>3.ทดลอง TensorFlow อย่างง่าย (สำเร็จ)</t>
+  </si>
+  <si>
+    <t>-code อยู่ใน Research/lab/DeepLearning1.py</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -67,7 +74,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -77,6 +84,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -108,16 +121,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -394,11 +408,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -457,6 +471,16 @@
         <v>10</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>

</xml_diff>

<commit_message>
code basic_classification and update workSheet
</commit_message>
<xml_diff>
--- a/workSheet.xlsx
+++ b/workSheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F53C2CA4-BD42-4224-B6C1-603BB40001B6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{171B5496-170A-433A-8F30-96AB0548D36E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3105" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>วันที่</t>
   </si>
@@ -58,7 +58,13 @@
     <t>3.ทดลอง TensorFlow อย่างง่าย (สำเร็จ)</t>
   </si>
   <si>
-    <t>-code อยู่ใน Research/lab/DeepLearning1.py</t>
+    <t>4.ทดลองแยกภาพด้วย TensorFlow ใช้ dataSet : MNIST</t>
+  </si>
+  <si>
+    <t>Path : Research/lab/DeepLearning1.py</t>
+  </si>
+  <si>
+    <t>Path : Research/lab/basic_classification_tShirtSneaker.py</t>
   </si>
 </sst>
 </file>
@@ -125,10 +131,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -423,11 +429,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -472,13 +478,23 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update workSheet and code basic_regression.py
</commit_message>
<xml_diff>
--- a/workSheet.xlsx
+++ b/workSheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6527DFFF-A64B-4574-B837-83F4D591571B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{317F5F2C-76A9-4FCA-9103-4F6FCBC1B385}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3105" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4155" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>วันที่</t>
   </si>
@@ -58,9 +58,6 @@
     <t>3.ทดลอง TensorFlow อย่างง่าย (สำเร็จ)</t>
   </si>
   <si>
-    <t>4.ทดลองแยกภาพด้วย TensorFlow ใช้ dataSet : MNIST</t>
-  </si>
-  <si>
     <t>Path : Research/lab/DeepLearning1.py</t>
   </si>
   <si>
@@ -68,6 +65,36 @@
   </si>
   <si>
     <t>hohohoho</t>
+  </si>
+  <si>
+    <t>4.ทดลองฝึกแยกภาพด้วย TensorFlow ใช้ dataSet : MNIST</t>
+  </si>
+  <si>
+    <t>5.ทดลองฝึกแยกตัวอักษรด้วย TensorFlow ใช้ dataSet : IMDB</t>
+  </si>
+  <si>
+    <t>6.ทดลอง Plot graph</t>
+  </si>
+  <si>
+    <t>Path : Research/lab/basic_classification_text.py</t>
+  </si>
+  <si>
+    <t>Path : Research/lab/tutorial_plotGraph.py</t>
+  </si>
+  <si>
+    <t>7.จ่ายงาน</t>
+  </si>
+  <si>
+    <t>7.1)Research</t>
+  </si>
+  <si>
+    <t>7.1.1)tensorflow</t>
+  </si>
+  <si>
+    <t>7.1.2)numpy</t>
+  </si>
+  <si>
+    <t>7.1.3)keras</t>
   </si>
 </sst>
 </file>
@@ -78,7 +105,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -418,27 +445,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="73.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="73.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.75" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -449,7 +476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -457,7 +484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -465,42 +492,87 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>14</v>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>